<commit_message>
Added additional tests and updated bug report
</commit_message>
<xml_diff>
--- a/Frontend-Tests-Swag-Labs/Swag Labs Bug Report.xlsx
+++ b/Frontend-Tests-Swag-Labs/Swag Labs Bug Report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="101">
   <si>
     <t>Category</t>
   </si>
@@ -288,7 +288,48 @@
     <t>Low</t>
   </si>
   <si>
-    <t>User reported bug.</t>
+    <t>Users aware we know of bug.</t>
+  </si>
+  <si>
+    <t>#011</t>
+  </si>
+  <si>
+    <t>PRODUCT - Description failing to render</t>
+  </si>
+  <si>
+    <t>Product descriptions are failing to display correctly on product pages.</t>
+  </si>
+  <si>
+    <t>1. While on inventory page, press on a product name</t>
+  </si>
+  <si>
+    <t>Same product description from inventory page to display</t>
+  </si>
+  <si>
+    <t>Displays error message saying failing to render</t>
+  </si>
+  <si>
+    <t>#012</t>
+  </si>
+  <si>
+    <t>CART - Failing to display after adding broken item</t>
+  </si>
+  <si>
+    <t>User is able to add a broken item which causes cart page to break when navigating to cart</t>
+  </si>
+  <si>
+    <t>https://www.saucedemo.com/cart.html</t>
+  </si>
+  <si>
+    <t>1. While on inventory page, press on the fleece jacket
+2. Product page displays broken item, press add to cart
+3. Navigate to cart page</t>
+  </si>
+  <si>
+    <t>Error should display that cannot add broken item</t>
+  </si>
+  <si>
+    <t>Item displays as added in cart and navigating to cart shows broken page</t>
   </si>
 </sst>
 </file>
@@ -2062,8 +2103,282 @@
         <v>87</v>
       </c>
     </row>
+    <row r="162">
+      <c r="A162" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B163" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C163" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="7"/>
+      <c r="B164" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C164" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="7"/>
+      <c r="B165" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C165" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="8"/>
+      <c r="B166" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C166" s="9">
+        <v>45873.0</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B167" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C167" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="7"/>
+      <c r="B168" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C168" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="8"/>
+      <c r="B169" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C169" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B170" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C170" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="7"/>
+      <c r="B171" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C171" s="6" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="8"/>
+      <c r="B172" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C172" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B173" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C173" s="23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="8"/>
+      <c r="B174" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C174" s="23" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B175" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C175" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B180" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C180" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="7"/>
+      <c r="B181" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C181" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="7"/>
+      <c r="B182" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C182" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="8"/>
+      <c r="B183" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C183" s="9">
+        <v>45873.0</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B184" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C184" s="6" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="7"/>
+      <c r="B185" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C185" s="10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="8"/>
+      <c r="B186" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C186" s="12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B187" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C187" s="6" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="7"/>
+      <c r="B188" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C188" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="8"/>
+      <c r="B189" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C189" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="B190" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C190" s="23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="8"/>
+      <c r="B191" s="22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C191" s="23" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B192" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C192" s="6"/>
+    </row>
   </sheetData>
-  <mergeCells count="40">
+  <mergeCells count="48">
     <mergeCell ref="A3:A6"/>
     <mergeCell ref="A7:A9"/>
     <mergeCell ref="A10:A12"/>
@@ -2078,32 +2393,40 @@
     <mergeCell ref="A45:A46"/>
     <mergeCell ref="A51:A54"/>
     <mergeCell ref="A55:A57"/>
-    <mergeCell ref="A90:A92"/>
+    <mergeCell ref="A58:A60"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A67:A70"/>
+    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="A74:A76"/>
+    <mergeCell ref="A77:A78"/>
     <mergeCell ref="A83:A86"/>
     <mergeCell ref="A87:A89"/>
-    <mergeCell ref="A58:A60"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="A74:A76"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="A67:A70"/>
-    <mergeCell ref="A71:A73"/>
+    <mergeCell ref="A90:A92"/>
     <mergeCell ref="A93:A94"/>
-    <mergeCell ref="A106:A108"/>
     <mergeCell ref="A99:A102"/>
     <mergeCell ref="A103:A105"/>
+    <mergeCell ref="A106:A108"/>
     <mergeCell ref="A109:A110"/>
-    <mergeCell ref="A122:A124"/>
     <mergeCell ref="A115:A118"/>
     <mergeCell ref="A119:A121"/>
-    <mergeCell ref="A154:A156"/>
-    <mergeCell ref="A157:A158"/>
+    <mergeCell ref="A122:A124"/>
     <mergeCell ref="A125:A126"/>
-    <mergeCell ref="A138:A140"/>
     <mergeCell ref="A131:A134"/>
     <mergeCell ref="A135:A137"/>
+    <mergeCell ref="A138:A140"/>
+    <mergeCell ref="A170:A172"/>
+    <mergeCell ref="A173:A174"/>
+    <mergeCell ref="A187:A189"/>
+    <mergeCell ref="A190:A191"/>
+    <mergeCell ref="A180:A183"/>
+    <mergeCell ref="A184:A186"/>
     <mergeCell ref="A141:A142"/>
     <mergeCell ref="A147:A150"/>
     <mergeCell ref="A151:A153"/>
+    <mergeCell ref="A154:A156"/>
+    <mergeCell ref="A157:A158"/>
+    <mergeCell ref="A163:A166"/>
+    <mergeCell ref="A167:A169"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="C8"/>
@@ -2116,7 +2439,9 @@
     <hyperlink r:id="rId8" ref="C120"/>
     <hyperlink r:id="rId9" ref="C136"/>
     <hyperlink r:id="rId10" ref="C152"/>
+    <hyperlink r:id="rId11" ref="C168"/>
+    <hyperlink r:id="rId12" ref="C185"/>
   </hyperlinks>
-  <drawing r:id="rId11"/>
+  <drawing r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>